<commit_message>
haploid estimates brought in one folder
</commit_message>
<xml_diff>
--- a/TraitAnalyses201003/ReorderPedigree/Ped_in_Order_754_Individuals.xlsx
+++ b/TraitAnalyses201003/ReorderPedigree/Ped_in_Order_754_Individuals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4400" yWindow="0" windowWidth="28580" windowHeight="14800" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="25360" windowHeight="15000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ped_in_Order_754_Individuals.cs" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5852" uniqueCount="920">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5854" uniqueCount="922">
   <si>
     <t>fndRow</t>
   </si>
@@ -2717,9 +2717,6 @@
     <t>544 to 787</t>
   </si>
   <si>
-    <t>243 plots?</t>
-  </si>
-  <si>
     <t>789-866</t>
   </si>
   <si>
@@ -2781,6 +2778,15 @@
   </si>
   <si>
     <t>GP for 5</t>
+  </si>
+  <si>
+    <t>haploid level</t>
+  </si>
+  <si>
+    <t>row #</t>
+  </si>
+  <si>
+    <t>244 plots?</t>
   </si>
 </sst>
 </file>
@@ -2898,8 +2904,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2937,7 +2945,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2950,6 +2958,7 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2962,6 +2971,7 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -49216,7 +49226,7 @@
         <v>702</v>
       </c>
       <c r="N708">
-        <f t="shared" ref="N708:N771" si="35">IF(L708=O708,0,1)</f>
+        <f t="shared" ref="N708:N757" si="35">IF(L708=O708,0,1)</f>
         <v>0</v>
       </c>
       <c r="O708" t="s">
@@ -54994,10 +55004,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E21"/>
+      <selection activeCell="B9" sqref="B9:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -55007,7 +55017,7 @@
     <col min="4" max="4" width="63" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="C1" s="3" t="s">
         <v>870</v>
       </c>
@@ -55015,7 +55025,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:8">
       <c r="C2" s="5">
         <v>1</v>
       </c>
@@ -55023,7 +55033,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:8">
       <c r="C3" s="7">
         <v>2</v>
       </c>
@@ -55031,7 +55041,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:8">
       <c r="C4" s="7">
         <v>3</v>
       </c>
@@ -55039,7 +55049,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:8">
       <c r="C5" s="7">
         <v>4</v>
       </c>
@@ -55047,7 +55057,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:8">
       <c r="C6" s="8">
         <v>5</v>
       </c>
@@ -55055,53 +55065,59 @@
         <v>874</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>877</v>
       </c>
       <c r="B8" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C8" t="s">
         <v>870</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="G8" t="s">
+        <v>919</v>
+      </c>
+      <c r="H8" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>878</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="C9" t="s">
         <v>880</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>879</v>
       </c>
       <c r="B10" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C10" t="s">
         <v>883</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>881</v>
       </c>
       <c r="B11" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="C11" t="s">
         <v>884</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:8">
       <c r="B12" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C12" t="s">
         <v>885</v>
@@ -55110,78 +55126,89 @@
         <v>891</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>882</v>
       </c>
       <c r="B13" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C13" t="s">
         <v>886</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="G13">
+        <f>104*2</f>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>887</v>
       </c>
       <c r="B14" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="C14" t="s">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>888</v>
       </c>
       <c r="B15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="C15" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>889</v>
       </c>
       <c r="B16" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C16" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="B17" t="s">
+        <v>908</v>
+      </c>
+      <c r="C17" t="s">
         <v>917</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="B17" t="s">
-        <v>909</v>
-      </c>
-      <c r="C17" t="s">
-        <v>918</v>
       </c>
       <c r="D17" t="s">
         <v>892</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>890</v>
       </c>
       <c r="B18" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="C18" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>918</v>
+      </c>
+      <c r="G18">
+        <v>439</v>
+      </c>
+      <c r="H18">
+        <f>439+208</f>
+        <v>647</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>897</v>
       </c>
       <c r="B19" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C19" t="s">
         <v>894</v>
@@ -55190,32 +55217,52 @@
         <v>893</v>
       </c>
       <c r="E19" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>921</v>
+      </c>
+      <c r="G19">
+        <f>(787-543)*2</f>
+        <v>488</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>788</v>
       </c>
       <c r="B20" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C20" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="D20" t="s">
         <v>895</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <f>647+486+2</f>
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B21" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C21" t="s">
         <v>896</v>
+      </c>
+      <c r="G21">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="G22">
+        <f>SUM(G13:G21)</f>
+        <v>1215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>